<commit_message>
Move startup to startupBoard, comment color sensor for now
</commit_message>
<xml_diff>
--- a/doc/doc/pinout.xlsx
+++ b/doc/doc/pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\Documents\MCUXpressoIDE_11.5.1_7266\workspace\frdmkl25z\doc\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACF86CF-B64B-48A7-B3D8-2FA34B764EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060048B2-5F3E-421B-9AB5-76E6FD508AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
   <si>
     <t>PTA13</t>
   </si>
@@ -157,13 +157,46 @@
   </si>
   <si>
     <t>LOW</t>
+  </si>
+  <si>
+    <t>Merime HIGH, abychom dostali sirku pasma, aka barvu</t>
+  </si>
+  <si>
+    <t>PIN</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>ALT func</t>
+  </si>
+  <si>
+    <t>Dev. ID</t>
+  </si>
+  <si>
+    <t>FTM0_CH0</t>
+  </si>
+  <si>
+    <t>FTM0_CH2</t>
+  </si>
+  <si>
+    <t>FTM0_CH3</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>Pull Up</t>
+  </si>
+  <si>
+    <t>Pull Up/Down</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,8 +213,16 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,6 +232,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -324,42 +377,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -370,7 +393,70 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -653,271 +739,406 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:K22"/>
+  <dimension ref="B2:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="8" max="8" width="71.5703125" customWidth="1"/>
+    <col min="3" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" customWidth="1"/>
+    <col min="10" max="10" width="71.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+    <row r="2" spans="2:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
-      <c r="H2" s="17" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="9"/>
+      <c r="J2" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+    </row>
+    <row r="3" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="13"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="H3" s="15" t="s">
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="21"/>
+      <c r="J4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D5" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="H4" s="15" t="s">
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="21"/>
+      <c r="J5" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D6" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="H5" s="15"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="H6" s="16"/>
-    </row>
-    <row r="7" spans="2:11" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="18"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="2:13" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C10" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="3" t="s">
+      <c r="D10" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C11" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="3" t="s">
+      <c r="D11" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="23"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-    </row>
-    <row r="11" spans="2:11" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="2:13" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C15" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D15" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F15" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="25"/>
+      <c r="G18" s="26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="2" t="s">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="F20" s="25"/>
+      <c r="G20" s="26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="6" t="s">
+      <c r="F21" s="17"/>
+      <c r="G21" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="2:5" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B20" s="10" t="s">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="2:7" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="9"/>
+    </row>
+    <row r="24" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="13"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C25" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="8" t="s">
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="27" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C26" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="9"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="E21:E22"/>
+  <mergeCells count="6">
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="G25:G26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add minor color sensor interrupts, main sensor check
Not tested yet!
Need to verify...
Edit pinout table
</commit_message>
<xml_diff>
--- a/doc/doc/pinout.xlsx
+++ b/doc/doc/pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\Documents\MCUXpressoIDE_11.5.1_7266\workspace\frdmkl25z\doc\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060048B2-5F3E-421B-9AB5-76E6FD508AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB71BF9-CBA4-4127-A485-55099A911A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
   <si>
     <t>PTA13</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Right color sensor</t>
   </si>
   <si>
-    <t xml:space="preserve">PTC4 </t>
-  </si>
-  <si>
     <t>Center color sensor</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>S0, S2 TCS3200 pin</t>
   </si>
   <si>
-    <t>PTC3</t>
-  </si>
-  <si>
     <t>S1, S3 TCS3200 pin</t>
   </si>
   <si>
@@ -99,104 +93,122 @@
     <t>PTA5</t>
   </si>
   <si>
+    <t>PTD2</t>
+  </si>
+  <si>
+    <t>PTD3</t>
+  </si>
+  <si>
+    <t>Motory</t>
+  </si>
+  <si>
+    <t>Senzory</t>
+  </si>
+  <si>
+    <t>Laser</t>
+  </si>
+  <si>
+    <t>PTC11</t>
+  </si>
+  <si>
+    <t>PTC10</t>
+  </si>
+  <si>
+    <t>I2C1</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>https://os.mbed.com/platforms/KL25Z/</t>
+  </si>
+  <si>
+    <t>Uzitecne odkazy</t>
+  </si>
+  <si>
+    <t>Hallovky</t>
+  </si>
+  <si>
+    <t>PTA1</t>
+  </si>
+  <si>
+    <t>Left hall</t>
+  </si>
+  <si>
+    <t>Right hall</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>Merime HIGH, abychom dostali sirku pasma, aka barvu</t>
+  </si>
+  <si>
+    <t>PIN</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>ALT func</t>
+  </si>
+  <si>
+    <t>Dev. ID</t>
+  </si>
+  <si>
+    <t>FTM0_CH0</t>
+  </si>
+  <si>
+    <t>FTM0_CH2</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>Pull Up</t>
+  </si>
+  <si>
+    <t>Pull Up/Down</t>
+  </si>
+  <si>
+    <t>OpenSDA</t>
+  </si>
+  <si>
+    <t>PTA0</t>
+  </si>
+  <si>
+    <t>RX</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>UART0</t>
+  </si>
+  <si>
+    <t>PTC4</t>
+  </si>
+  <si>
+    <t>PTC5</t>
+  </si>
+  <si>
     <t>PTD0</t>
   </si>
   <si>
-    <t>PTD2</t>
-  </si>
-  <si>
-    <t>PTD3</t>
-  </si>
-  <si>
-    <t>Motory</t>
-  </si>
-  <si>
-    <t>Senzory</t>
-  </si>
-  <si>
-    <t>Laser</t>
-  </si>
-  <si>
-    <t>PTC11</t>
-  </si>
-  <si>
-    <t>PTC10</t>
-  </si>
-  <si>
-    <t>I2C1</t>
-  </si>
-  <si>
-    <t>SDA</t>
-  </si>
-  <si>
-    <t>SCL</t>
-  </si>
-  <si>
-    <t>https://os.mbed.com/platforms/KL25Z/</t>
-  </si>
-  <si>
-    <t>Uzitecne odkazy</t>
-  </si>
-  <si>
-    <t>Hallovky</t>
-  </si>
-  <si>
-    <t>PTA1</t>
-  </si>
-  <si>
-    <t>PTA2</t>
-  </si>
-  <si>
-    <t>Left hall</t>
-  </si>
-  <si>
-    <t>Right hall</t>
-  </si>
-  <si>
-    <t>HIGH</t>
-  </si>
-  <si>
-    <t>LOW</t>
-  </si>
-  <si>
-    <t>Merime HIGH, abychom dostali sirku pasma, aka barvu</t>
-  </si>
-  <si>
-    <t>PIN</t>
-  </si>
-  <si>
-    <t>Device</t>
-  </si>
-  <si>
-    <t>ALT func</t>
-  </si>
-  <si>
-    <t>Dev. ID</t>
-  </si>
-  <si>
-    <t>FTM0_CH0</t>
-  </si>
-  <si>
-    <t>FTM0_CH2</t>
-  </si>
-  <si>
-    <t>FTM0_CH3</t>
-  </si>
-  <si>
-    <t>&gt;</t>
-  </si>
-  <si>
-    <t>Pull Up</t>
-  </si>
-  <si>
-    <t>Pull Up/Down</t>
+    <t>PTD1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +231,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -377,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -393,15 +413,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -414,50 +425,71 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -739,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:M26"/>
+  <dimension ref="A2:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,92 +786,92 @@
     <col min="10" max="10" width="71.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="9"/>
-      <c r="J2" s="14" t="s">
-        <v>36</v>
+    <row r="2" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="26"/>
+      <c r="J2" s="29" t="s">
+        <v>33</v>
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="13"/>
-      <c r="J3" s="15"/>
+    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="10"/>
+      <c r="J3" s="30"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="21"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="16"/>
       <c r="J4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="16"/>
       <c r="J5" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="18"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="13"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -848,65 +880,65 @@
       <c r="G7" s="1"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="2:13" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+    <row r="8" spans="1:13" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B8" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="26"/>
+    </row>
+    <row r="9" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="10"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="12" t="s">
+      <c r="D11" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E11" s="18"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -914,164 +946,167 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="2:13" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
+    <row r="13" spans="1:13" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B13" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="26"/>
+    </row>
+    <row r="14" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="32"/>
+      <c r="B15" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="E15" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="32"/>
+      <c r="B16" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
+      <c r="B17" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="E17" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="25" t="s">
+      <c r="G17" s="21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E18" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="20"/>
+      <c r="G18" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="25" t="s">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="20"/>
+      <c r="G19" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" s="26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="25"/>
-      <c r="G18" s="26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="25" t="s">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="25"/>
-      <c r="G19" s="26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="25" t="s">
+      <c r="D20" s="20"/>
+      <c r="E20" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="20"/>
+      <c r="G20" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="25"/>
-      <c r="G20" s="26" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="16" t="s">
+      <c r="D21" s="12"/>
+      <c r="E21" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F21" s="12"/>
+      <c r="G21" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1079,66 +1114,120 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="2:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
+    <row r="23" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B23" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="26"/>
+    </row>
+    <row r="24" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="9"/>
-    </row>
-    <row r="24" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="13"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="16" t="s">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="28"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="23"/>
+    </row>
+    <row r="28" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B28" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="26"/>
+    </row>
+    <row r="29" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" s="9"/>
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="G30:G31"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="B8:G8"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="B23:G23"/>
-    <mergeCell ref="G25:G26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Create control unit file. Replace wait with vTaskDelay
</commit_message>
<xml_diff>
--- a/doc/doc/pinout.xlsx
+++ b/doc/doc/pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\Documents\MCUXpressoIDE_11.5.1_7266\workspace\frdmkl25z\doc\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB71BF9-CBA4-4127-A485-55099A911A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58938509-60C3-47D2-974D-9A05C179AB32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -458,38 +458,38 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -773,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,15 +787,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
-      <c r="J2" s="29" t="s">
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="28"/>
+      <c r="J2" s="31" t="s">
         <v>33</v>
       </c>
       <c r="K2" s="4"/>
@@ -817,7 +817,7 @@
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="10"/>
-      <c r="J3" s="30"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
@@ -827,7 +827,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>8</v>
@@ -844,7 +844,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>7</v>
@@ -881,14 +881,14 @@
       <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:13" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="26"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="28"/>
     </row>
     <row r="9" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
@@ -907,7 +907,7 @@
       <c r="G9" s="10"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="15" t="s">
@@ -947,14 +947,14 @@
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:13" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="28"/>
     </row>
     <row r="14" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
@@ -973,7 +973,7 @@
       <c r="G14" s="10"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="19" t="s">
         <v>57</v>
       </c>
@@ -997,7 +997,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="19" t="s">
         <v>58</v>
       </c>
@@ -1018,7 +1018,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="19" t="s">
         <v>22</v>
       </c>
@@ -1115,14 +1115,14 @@
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="26"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="28"/>
     </row>
     <row r="24" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
@@ -1150,7 +1150,7 @@
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
       <c r="F25" s="20"/>
-      <c r="G25" s="22" t="s">
+      <c r="G25" s="24" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1164,17 +1164,17 @@
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
-      <c r="G26" s="23"/>
+      <c r="G26" s="25"/>
     </row>
     <row r="28" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="26"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="28"/>
     </row>
     <row r="29" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
@@ -1202,7 +1202,7 @@
       <c r="D30" s="15"/>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
-      <c r="G30" s="27" t="s">
+      <c r="G30" s="29" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1216,7 +1216,7 @@
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
-      <c r="G31" s="28"/>
+      <c r="G31" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Remove freertos, new pinout
Wel... You can build it, but many many changes. I am bad at commiting, sry
</commit_message>
<xml_diff>
--- a/doc/doc/pinout.xlsx
+++ b/doc/doc/pinout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\Documents\MCUXpressoIDE_11.5.1_7266\workspace\frdmkl25z\doc\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58938509-60C3-47D2-974D-9A05C179AB32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F72B905-190B-4712-9EDE-B8A849FA17C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="65">
   <si>
     <t>PTA13</t>
   </si>
@@ -87,9 +87,6 @@
     <t>IRQ</t>
   </si>
   <si>
-    <t>PTA4</t>
-  </si>
-  <si>
     <t>PTA5</t>
   </si>
   <si>
@@ -165,18 +162,12 @@
     <t>FTM0_CH0</t>
   </si>
   <si>
-    <t>FTM0_CH2</t>
-  </si>
-  <si>
     <t>&gt;</t>
   </si>
   <si>
     <t>Pull Up</t>
   </si>
   <si>
-    <t>Pull Up/Down</t>
-  </si>
-  <si>
     <t>OpenSDA</t>
   </si>
   <si>
@@ -201,7 +192,34 @@
     <t>PTD0</t>
   </si>
   <si>
-    <t>PTD1</t>
+    <t>FTM0_CH3</t>
+  </si>
+  <si>
+    <t>PTD4</t>
+  </si>
+  <si>
+    <t>FTM0_CH4</t>
+  </si>
+  <si>
+    <t>PWM</t>
+  </si>
+  <si>
+    <t>GPIO</t>
+  </si>
+  <si>
+    <t>PTA2</t>
+  </si>
+  <si>
+    <t>GPIOC, 4</t>
+  </si>
+  <si>
+    <t>GPIOC, 5</t>
+  </si>
+  <si>
+    <t>GPIOA, 0</t>
+  </si>
+  <si>
+    <t>GPIOA, 5</t>
   </si>
 </sst>
 </file>
@@ -461,35 +479,35 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -773,56 +791,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" style="32"/>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="4" width="19.42578125" customWidth="1"/>
     <col min="5" max="5" width="20.140625" customWidth="1"/>
     <col min="6" max="6" width="6.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="2"/>
     <col min="10" max="10" width="71.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="28"/>
-      <c r="J2" s="31" t="s">
-        <v>33</v>
+    <row r="2" spans="2:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="27"/>
+      <c r="J2" s="30" t="s">
+        <v>32</v>
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>44</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="10"/>
-      <c r="J3" s="32"/>
+      <c r="J3" s="31"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>2</v>
       </c>
@@ -835,11 +855,14 @@
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="16"/>
+      <c r="H4" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="J4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
         <v>0</v>
       </c>
@@ -852,11 +875,14 @@
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="16"/>
+      <c r="H5" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="J5" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
         <v>5</v>
       </c>
@@ -869,9 +895,12 @@
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="13"/>
+      <c r="H6" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -880,65 +909,71 @@
       <c r="G7" s="1"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:13" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="28"/>
-    </row>
-    <row r="9" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B8" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="27"/>
+    </row>
+    <row r="9" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="D9" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="E9" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>44</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="16" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H10" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E11" s="18"/>
       <c r="F11" s="15"/>
       <c r="G11" s="16" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H11" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -946,79 +981,76 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:13" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B13" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="28"/>
-    </row>
-    <row r="14" spans="1:13" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B13" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="27"/>
+    </row>
+    <row r="14" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="D14" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="E14" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>44</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" s="20" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G15" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C16" s="20" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>17</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G16" s="21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="19" t="s">
         <v>22</v>
       </c>
@@ -1026,27 +1058,27 @@
         <v>12</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>17</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G17" s="21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="19" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="C18" s="20" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="E18" s="20" t="s">
         <v>18</v>
@@ -1055,16 +1087,19 @@
       <c r="G18" s="21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>18</v>
@@ -1073,40 +1108,53 @@
       <c r="G19" s="21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="20"/>
+      <c r="D20" s="20" t="s">
+        <v>61</v>
+      </c>
       <c r="E20" s="20" t="s">
         <v>17</v>
       </c>
       <c r="F20" s="20"/>
       <c r="G20" s="21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="12"/>
+      <c r="D21" s="12" t="s">
+        <v>62</v>
+      </c>
       <c r="E21" s="12" t="s">
         <v>17</v>
       </c>
       <c r="F21" s="12"/>
       <c r="G21" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="H21" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1114,109 +1162,109 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B23" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="28"/>
-    </row>
-    <row r="24" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B23" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="27"/>
+    </row>
+    <row r="24" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="D24" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="E24" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>44</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="10"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
       <c r="F25" s="20"/>
-      <c r="G25" s="24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
-      <c r="G26" s="25"/>
-    </row>
-    <row r="28" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B28" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="28"/>
-    </row>
-    <row r="29" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="G26" s="24"/>
+    </row>
+    <row r="28" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B28" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="27"/>
+    </row>
+    <row r="29" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="D29" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="E29" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>44</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="10"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D30" s="15"/>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
-      <c r="G30" s="29" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G30" s="28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="17" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
-      <c r="G31" s="30"/>
+      <c r="G31" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Prepare input capture for color sensor, template for interrupts with comments
</commit_message>
<xml_diff>
--- a/doc/doc/pinout.xlsx
+++ b/doc/doc/pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\Documents\MCUXpressoIDE_11.5.1_7266\workspace\frdmkl25z\doc\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F72B905-190B-4712-9EDE-B8A849FA17C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9CEC90-5470-4229-B93D-9877CA2794FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -479,35 +479,35 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -795,34 +795,34 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="32"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="4" width="19.42578125" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="2"/>
-    <col min="10" max="10" width="71.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="23"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+    <col min="3" max="4" width="19.44140625" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" customWidth="1"/>
+    <col min="6" max="6" width="6.109375" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" style="2"/>
+    <col min="10" max="10" width="71.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
+    <row r="2" spans="2:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="27"/>
-      <c r="J2" s="30" t="s">
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="28"/>
+      <c r="J2" s="31" t="s">
         <v>32</v>
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
         <v>40</v>
       </c>
@@ -837,12 +837,12 @@
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="10"/>
-      <c r="J3" s="31"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
         <v>2</v>
       </c>
@@ -862,7 +862,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" s="14" t="s">
         <v>0</v>
       </c>
@@ -882,7 +882,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
         <v>5</v>
       </c>
@@ -900,7 +900,7 @@
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -909,17 +909,17 @@
       <c r="G7" s="1"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="2:13" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="25" t="s">
+    <row r="8" spans="2:13" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="B8" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="27"/>
-    </row>
-    <row r="9" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="28"/>
+    </row>
+    <row r="9" spans="2:13" ht="18" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
         <v>40</v>
       </c>
@@ -935,7 +935,7 @@
       <c r="F9" s="9"/>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" s="22" t="s">
         <v>21</v>
       </c>
@@ -954,7 +954,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" s="17" t="s">
         <v>21</v>
       </c>
@@ -973,7 +973,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -981,17 +981,17 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="2:13" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B13" s="25" t="s">
+    <row r="13" spans="2:13" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="B13" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="27"/>
-    </row>
-    <row r="14" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="28"/>
+    </row>
+    <row r="14" spans="2:13" ht="18" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="s">
         <v>40</v>
       </c>
@@ -1007,7 +1007,7 @@
       <c r="F14" s="9"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="19" t="s">
         <v>54</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16" s="19" t="s">
         <v>56</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="19" t="s">
         <v>22</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="19" t="s">
         <v>48</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="19" t="s">
         <v>20</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="19" t="s">
         <v>52</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="11" t="s">
         <v>53</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1162,17 +1162,17 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B23" s="25" t="s">
+    <row r="23" spans="2:8" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="B23" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="27"/>
-    </row>
-    <row r="24" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="28"/>
+    </row>
+    <row r="24" spans="2:8" ht="18" x14ac:dyDescent="0.3">
       <c r="B24" s="8" t="s">
         <v>40</v>
       </c>
@@ -1188,7 +1188,7 @@
       <c r="F24" s="9"/>
       <c r="G24" s="10"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="19" t="s">
         <v>26</v>
       </c>
@@ -1198,11 +1198,11 @@
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
       <c r="F25" s="20"/>
-      <c r="G25" s="23" t="s">
+      <c r="G25" s="24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="11" t="s">
         <v>27</v>
       </c>
@@ -1212,19 +1212,19 @@
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
-      <c r="G26" s="24"/>
-    </row>
-    <row r="28" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="B28" s="25" t="s">
+      <c r="G26" s="25"/>
+    </row>
+    <row r="28" spans="2:8" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="B28" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="27"/>
-    </row>
-    <row r="29" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="28"/>
+    </row>
+    <row r="29" spans="2:8" ht="18" x14ac:dyDescent="0.3">
       <c r="B29" s="8" t="s">
         <v>40</v>
       </c>
@@ -1240,7 +1240,7 @@
       <c r="F29" s="9"/>
       <c r="G29" s="10"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" s="14" t="s">
         <v>34</v>
       </c>
@@ -1250,11 +1250,11 @@
       <c r="D30" s="15"/>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
-      <c r="G30" s="28" t="s">
+      <c r="G30" s="29" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" s="17" t="s">
         <v>60</v>
       </c>
@@ -1264,7 +1264,7 @@
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
-      <c r="G31" s="29"/>
+      <c r="G31" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Input capture is not working
</commit_message>
<xml_diff>
--- a/doc/doc/pinout.xlsx
+++ b/doc/doc/pinout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\Documents\MCUXpressoIDE_11.5.1_7266\workspace\frdmkl25z\doc\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9CEC90-5470-4229-B93D-9877CA2794FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA1FDBF-BAC6-4C96-95F4-04737D09B01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -171,9 +171,6 @@
     <t>OpenSDA</t>
   </si>
   <si>
-    <t>PTA0</t>
-  </si>
-  <si>
     <t>RX</t>
   </si>
   <si>
@@ -216,10 +213,13 @@
     <t>GPIOC, 5</t>
   </si>
   <si>
-    <t>GPIOA, 0</t>
-  </si>
-  <si>
     <t>GPIOA, 5</t>
+  </si>
+  <si>
+    <t>PTA4</t>
+  </si>
+  <si>
+    <t>GPIOA, 4</t>
   </si>
 </sst>
 </file>
@@ -524,6 +524,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>182515</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>198122</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>50690</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C6BBB13-0B19-1561-0017-DC6E4E4FAE3E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7805057" y="1935115"/>
+          <a:ext cx="5107579" cy="3362489"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -791,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -856,7 +905,7 @@
       <c r="F4" s="15"/>
       <c r="G4" s="16"/>
       <c r="H4" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>4</v>
@@ -876,7 +925,7 @@
       <c r="F5" s="15"/>
       <c r="G5" s="16"/>
       <c r="H5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>31</v>
@@ -896,7 +945,7 @@
       <c r="F6" s="12"/>
       <c r="G6" s="13"/>
       <c r="H6" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J6" s="5"/>
     </row>
@@ -1009,7 +1058,7 @@
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>10</v>
@@ -1032,13 +1081,13 @@
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="20" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>17</v>
@@ -1058,7 +1107,7 @@
         <v>12</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>17</v>
@@ -1072,13 +1121,13 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="19" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="C18" s="20" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E18" s="20" t="s">
         <v>18</v>
@@ -1099,7 +1148,7 @@
         <v>14</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>18</v>
@@ -1114,13 +1163,13 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>15</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E20" s="20" t="s">
         <v>17</v>
@@ -1130,18 +1179,18 @@
         <v>37</v>
       </c>
       <c r="H20" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>17</v>
@@ -1151,7 +1200,7 @@
         <v>38</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
@@ -1245,21 +1294,21 @@
         <v>34</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D30" s="15"/>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
       <c r="G30" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -1279,5 +1328,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>